<commit_message>
added images and cleaned notebbok
</commit_message>
<xml_diff>
--- a/ada.xlsx
+++ b/ada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EPFL\Courses\ADA\Project\P3\ada-2020-project-milestone-p3-p3_gyc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62574A4-F73C-410D-BBB2-BDF392AFF809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9BB8F7-DE17-41AF-9499-AB494FDF65D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="7995" windowWidth="21600" windowHeight="11385" xr2:uid="{83E75853-4D8B-4CBD-AC96-DDC4324C732E}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12735" xr2:uid="{83E75853-4D8B-4CBD-AC96-DDC4324C732E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="54">
   <si>
     <t>Classifier</t>
   </si>
@@ -171,18 +171,6 @@
   </si>
   <si>
     <t>SVM, sigmoid kernel, regularizer = 1</t>
-  </si>
-  <si>
-    <t>linear SVC, regularizer = 0.001</t>
-  </si>
-  <si>
-    <t>linear SVC, regularizer = 0.01</t>
-  </si>
-  <si>
-    <t>linear SVC, regularizer = 0.1</t>
-  </si>
-  <si>
-    <t>linear SVC, regularizer = 1</t>
   </si>
   <si>
     <t>KNN 1 neighbor</t>
@@ -520,6 +508,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,9 +518,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0578A1-0DEC-42A8-BBA6-2629203F1EDF}">
-  <dimension ref="C1:O63"/>
+  <dimension ref="C1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,18 +855,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="31"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="3:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C2" s="17" t="s">
@@ -1104,7 +1092,7 @@
         <v>0.77</v>
       </c>
       <c r="G12" s="11">
-        <v>7.6999999999999999E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="H12" s="12">
         <v>0.78</v>
@@ -1153,7 +1141,7 @@
         <v>0.91</v>
       </c>
       <c r="G15" s="10">
-        <v>0.22900000000000001</v>
+        <v>0.245</v>
       </c>
       <c r="H15" s="12">
         <v>0.91</v>
@@ -1167,62 +1155,70 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="2">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="C16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="H16" s="8">
         <v>0.92</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="I16" s="7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.76</v>
+      </c>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F18" s="3">
         <v>0.93</v>
       </c>
-      <c r="G17" s="7">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0.92</v>
-      </c>
-      <c r="I17" s="7">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0.76</v>
-      </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.91</v>
-      </c>
+      <c r="G18" s="3">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -1234,32 +1230,44 @@
       <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.93</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.93</v>
+      <c r="D20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="11">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.53</v>
+      </c>
+      <c r="G20" s="11">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0.63900000000000001</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="C21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G21" s="9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.63900000000000001</v>
+      </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="O21" s="1"/>
@@ -1268,19 +1276,19 @@
       <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="11">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0.53</v>
-      </c>
-      <c r="G22" s="11">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="D22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G22" s="9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H22" s="6">
         <v>0.63900000000000001</v>
       </c>
       <c r="I22" s="16"/>
@@ -1292,16 +1300,16 @@
         <v>11</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" s="9">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F23" s="9">
-        <v>0.55600000000000005</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="G23" s="9">
-        <v>5.7000000000000002E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H23" s="6">
         <v>0.63900000000000001</v>
@@ -1315,19 +1323,19 @@
         <v>11</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" s="9">
-        <v>5.7000000000000002E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F24" s="9">
-        <v>0.56000000000000005</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="G24" s="9">
-        <v>5.6000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H24" s="6">
-        <v>0.63900000000000001</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
@@ -1338,19 +1346,19 @@
         <v>11</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="9">
-        <v>2.5000000000000001E-2</v>
+        <v>50</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1.6E-2</v>
       </c>
       <c r="F25" s="9">
-        <v>0.57599999999999996</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="G25" s="9">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H25" s="6">
-        <v>0.63900000000000001</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
@@ -1361,19 +1369,19 @@
         <v>11</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="9">
-        <v>5.6000000000000001E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F26" s="9">
-        <v>0.58699999999999997</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="G26" s="9">
         <v>5.5E-2</v>
       </c>
       <c r="H26" s="6">
-        <v>0.63700000000000001</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
@@ -1384,19 +1392,19 @@
         <v>11</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="34">
+        <v>52</v>
+      </c>
+      <c r="E27" s="9">
         <v>1.6E-2</v>
       </c>
       <c r="F27" s="9">
-        <v>0.58499999999999996</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="G27" s="9">
-        <v>5.7000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H27" s="6">
-        <v>0.64500000000000002</v>
+        <v>0.64</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
@@ -1406,441 +1414,408 @@
       <c r="C28" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="9">
-        <v>4.7E-2</v>
-      </c>
-      <c r="F28" s="9">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="G28" s="9">
-        <v>5.5E-2</v>
-      </c>
-      <c r="H28" s="6">
-        <v>0.64100000000000001</v>
+      <c r="D28" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.65</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F29" s="9">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="G29" s="9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H29" s="6">
-        <v>0.64</v>
-      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0</v>
-      </c>
-      <c r="F30" s="13">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="G30" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="H30" s="8">
-        <v>0.65</v>
-      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="O31" s="1"/>
+      <c r="C31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F31" s="20">
+        <v>0.51</v>
+      </c>
+      <c r="G31" s="20">
+        <v>3.9E-2</v>
+      </c>
+      <c r="H31" s="21">
+        <v>0.54700000000000004</v>
+      </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="16"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="O32" s="1"/>
+      <c r="C32" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="23">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F32" s="23">
+        <v>0.51</v>
+      </c>
+      <c r="G32" s="23">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H32" s="24">
+        <v>0.61</v>
+      </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C33" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="20">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F33" s="20">
+      <c r="C33" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="23">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F33" s="23">
+        <v>0.51</v>
+      </c>
+      <c r="G33" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H33" s="24">
+        <v>0.59399999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="26">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F34" s="26">
+        <v>0.51</v>
+      </c>
+      <c r="G34" s="26">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H34" s="27">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="2"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="20">
+        <v>0</v>
+      </c>
+      <c r="F36" s="20">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G36" s="20">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H36" s="21">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="G37" s="23">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H37" s="24">
         <v>0.505</v>
       </c>
-      <c r="G33" s="20">
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="23">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F38" s="23">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="G38" s="23">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H38" s="24">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="26">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F39" s="26">
+        <v>0.498</v>
+      </c>
+      <c r="G39" s="26">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H39" s="27">
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="20">
+        <v>0</v>
+      </c>
+      <c r="F41" s="20">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="G41" s="20">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H41" s="21">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="23">
+        <v>0</v>
+      </c>
+      <c r="F42" s="23">
+        <v>0.51</v>
+      </c>
+      <c r="G42" s="23">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H42" s="24">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="23">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="G43" s="23">
         <v>3.1E-2</v>
       </c>
-      <c r="H33" s="21">
-        <v>0.501</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="23">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="F34" s="23">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="G34" s="23">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="H34" s="24">
-        <v>0.499</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="23">
-        <v>0.03</v>
-      </c>
-      <c r="F35" s="23">
-        <v>0.498</v>
-      </c>
-      <c r="G35" s="23">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="H35" s="24">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="26">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="F36" s="26">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="G36" s="26">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H36" s="27">
-        <v>0.502</v>
-      </c>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="20">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F37" s="20">
-        <v>0.51</v>
-      </c>
-      <c r="G37" s="20">
-        <v>3.9E-2</v>
-      </c>
-      <c r="H37" s="21">
-        <v>0.54700000000000004</v>
-      </c>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C38" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="23">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="F38" s="23">
-        <v>0.51</v>
-      </c>
-      <c r="G38" s="23">
-        <v>4.7E-2</v>
-      </c>
-      <c r="H38" s="24">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E39" s="23">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F39" s="23">
-        <v>0.51</v>
-      </c>
-      <c r="G39" s="23">
-        <v>0.05</v>
-      </c>
-      <c r="H39" s="24">
-        <v>0.59399999999999997</v>
-      </c>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="26">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F40" s="26">
-        <v>0.51</v>
-      </c>
-      <c r="G40" s="26">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H40" s="27">
-        <v>0.60499999999999998</v>
-      </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="20">
-        <v>0</v>
-      </c>
-      <c r="F42" s="20">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="G42" s="20">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H42" s="21">
+      <c r="H43" s="24">
         <v>0.51500000000000001</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="23">
-        <v>0</v>
-      </c>
-      <c r="F43" s="23">
-        <v>0.47699999999999998</v>
-      </c>
-      <c r="G43" s="23">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H43" s="24">
-        <v>0.505</v>
-      </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="O43" s="1"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="23">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F44" s="23">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="G44" s="23">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H44" s="24">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="16"/>
+      <c r="D44" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="26">
+        <v>0</v>
+      </c>
+      <c r="F44" s="26">
+        <v>0.48</v>
+      </c>
+      <c r="G44" s="26">
+        <v>3.1E-2</v>
+      </c>
+      <c r="H44" s="27">
+        <v>0.50600000000000001</v>
+      </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="26">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F45" s="26">
-        <v>0.498</v>
-      </c>
-      <c r="G45" s="26">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H45" s="27">
-        <v>0.51400000000000001</v>
-      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="C46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="20">
+        <v>0</v>
+      </c>
+      <c r="F46" s="20">
+        <v>0.52</v>
+      </c>
+      <c r="G46" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="H46" s="21">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="20">
-        <v>0</v>
-      </c>
-      <c r="F47" s="20">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="G47" s="20">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="H47" s="21">
-        <v>0.48399999999999999</v>
-      </c>
+      <c r="D47" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="23">
+        <v>0</v>
+      </c>
+      <c r="F47" s="23">
+        <v>0.52</v>
+      </c>
+      <c r="G47" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="H47" s="24">
+        <v>0.44</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E48" s="23">
         <v>0</v>
       </c>
       <c r="F48" s="23">
+        <v>0.52</v>
+      </c>
+      <c r="G48" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="H48" s="24">
         <v>0.51</v>
       </c>
-      <c r="G48" s="23">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="H48" s="24">
-        <v>0.498</v>
-      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="23">
-        <v>0</v>
-      </c>
-      <c r="F49" s="23">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="G49" s="23">
-        <v>3.1E-2</v>
-      </c>
-      <c r="H49" s="24">
-        <v>0.51500000000000001</v>
-      </c>
+      <c r="C49" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="26">
+        <v>0</v>
+      </c>
+      <c r="F49" s="26">
+        <v>0.52</v>
+      </c>
+      <c r="G49" s="26">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H49" s="27">
+        <v>0.54</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C50" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="26">
-        <v>0</v>
-      </c>
-      <c r="F50" s="26">
-        <v>0.48</v>
-      </c>
-      <c r="G50" s="26">
-        <v>3.1E-2</v>
-      </c>
-      <c r="H50" s="27">
-        <v>0.50600000000000001</v>
-      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="2"/>
@@ -1849,153 +1824,53 @@
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C52" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E52" s="20">
-        <v>0</v>
-      </c>
-      <c r="F52" s="20">
-        <v>0.52</v>
-      </c>
-      <c r="G52" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="H52" s="21">
-        <v>0.48399999999999999</v>
-      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C53" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" s="23">
-        <v>0</v>
-      </c>
-      <c r="F53" s="23">
-        <v>0.52</v>
-      </c>
-      <c r="G53" s="23">
-        <v>0.03</v>
-      </c>
-      <c r="H53" s="24">
-        <v>0.44</v>
-      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C54" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E54" s="23">
-        <v>0</v>
-      </c>
-      <c r="F54" s="23">
-        <v>0.52</v>
-      </c>
-      <c r="G54" s="23">
-        <v>0.03</v>
-      </c>
-      <c r="H54" s="24">
-        <v>0.51</v>
-      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C55" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" s="26">
-        <v>0</v>
-      </c>
-      <c r="F55" s="26">
-        <v>0.52</v>
-      </c>
-      <c r="G55" s="26">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H55" s="27">
-        <v>0.54</v>
-      </c>
+      <c r="C55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2152,14 +2027,14 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -2892,14 +2767,14 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="33" t="s">
+      <c r="J28" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>

</xml_diff>